<commit_message>
Redid placement and did layout, need to fix DRC
</commit_message>
<xml_diff>
--- a/CBU-PCB-BOM.xlsx
+++ b/CBU-PCB-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\CBU-PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F68941-92D6-4BA8-B63B-3808C35B0CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB50D5F1-2F60-4F8E-824A-0D3409C1D1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B4210671-1C10-43EA-9025-D3AE3D76F5F5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B4210671-1C10-43EA-9025-D3AE3D76F5F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="152">
   <si>
     <t>Ceramic Capacitor 0805</t>
   </si>
@@ -489,6 +489,9 @@
   </si>
   <si>
     <t>Resistor 0603</t>
+  </si>
+  <si>
+    <t>In cart?</t>
   </si>
 </sst>
 </file>
@@ -533,9 +536,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -852,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE061555-1CA7-4351-BAE9-68B383692A6F}">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="G21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -867,14 +869,14 @@
     <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.88671875" customWidth="1"/>
     <col min="11" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -911,8 +913,11 @@
       <c r="L1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -939,7 +944,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -966,7 +971,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -993,7 +998,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1022,18 +1027,21 @@
       <c r="I5" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5">
         <v>0.13</v>
       </c>
       <c r="L5">
         <f t="shared" ref="L5:L42" si="1">K5*G5</f>
         <v>0.39</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1060,7 +1068,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1089,7 +1097,7 @@
       <c r="I7" t="s">
         <v>105</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="1" t="s">
         <v>106</v>
       </c>
       <c r="K7">
@@ -1100,7 +1108,7 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1129,7 +1137,7 @@
       <c r="I8" t="s">
         <v>109</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="1" t="s">
         <v>108</v>
       </c>
       <c r="K8">
@@ -1140,7 +1148,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1169,7 +1177,7 @@
       <c r="I9" t="s">
         <v>111</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="1" t="s">
         <v>110</v>
       </c>
       <c r="K9">
@@ -1180,7 +1188,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1209,7 +1217,7 @@
       <c r="I10" t="s">
         <v>113</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="1" t="s">
         <v>112</v>
       </c>
       <c r="K10">
@@ -1220,7 +1228,7 @@
         <v>2.0999999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1249,7 +1257,7 @@
       <c r="I11" t="s">
         <v>114</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="1" t="s">
         <v>115</v>
       </c>
       <c r="K11">
@@ -1260,7 +1268,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1287,7 +1295,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1316,7 +1324,7 @@
       <c r="I13" t="s">
         <v>116</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="1" t="s">
         <v>118</v>
       </c>
       <c r="K13">
@@ -1327,7 +1335,7 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1353,7 +1361,7 @@
       <c r="I14" t="s">
         <v>18</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="1" t="s">
         <v>117</v>
       </c>
       <c r="K14">
@@ -1364,7 +1372,7 @@
         <v>13.799999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1390,7 +1398,7 @@
       <c r="I15" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" s="1" t="s">
         <v>120</v>
       </c>
       <c r="K15">
@@ -1401,7 +1409,7 @@
         <v>3.5100000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>742792042</v>
       </c>
@@ -1427,7 +1435,7 @@
       <c r="I16">
         <v>742792042</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="1" t="s">
         <v>121</v>
       </c>
       <c r="K16">
@@ -1488,7 +1496,7 @@
       <c r="I18">
         <v>901481104</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J18" s="1" t="s">
         <v>122</v>
       </c>
       <c r="K18">
@@ -1525,7 +1533,7 @@
       <c r="I19" t="s">
         <v>28</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="J19" s="1" t="s">
         <v>146</v>
       </c>
       <c r="K19">
@@ -1562,7 +1570,7 @@
       <c r="I20">
         <v>1714955</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="J20" s="1" t="s">
         <v>147</v>
       </c>
       <c r="K20">
@@ -1599,7 +1607,7 @@
       <c r="I21" t="s">
         <v>33</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="J21" s="1" t="s">
         <v>148</v>
       </c>
       <c r="K21">
@@ -1717,7 +1725,7 @@
       <c r="I25" t="s">
         <v>124</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="J25" s="1" t="s">
         <v>123</v>
       </c>
       <c r="K25">
@@ -1865,7 +1873,7 @@
       <c r="I30" t="s">
         <v>131</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="J30" s="1" t="s">
         <v>130</v>
       </c>
       <c r="K30">
@@ -1905,7 +1913,7 @@
       <c r="I31" t="s">
         <v>133</v>
       </c>
-      <c r="J31" s="2" t="s">
+      <c r="J31" s="1" t="s">
         <v>134</v>
       </c>
       <c r="K31">
@@ -1945,7 +1953,7 @@
       <c r="I32" t="s">
         <v>137</v>
       </c>
-      <c r="J32" s="2" t="s">
+      <c r="J32" s="1" t="s">
         <v>140</v>
       </c>
       <c r="K32">
@@ -1985,7 +1993,7 @@
       <c r="I33" t="s">
         <v>138</v>
       </c>
-      <c r="J33" s="2" t="s">
+      <c r="J33" s="1" t="s">
         <v>139</v>
       </c>
       <c r="K33">
@@ -2022,7 +2030,7 @@
       <c r="I34" t="s">
         <v>44</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="J34" s="1" t="s">
         <v>141</v>
       </c>
       <c r="K34">
@@ -2059,7 +2067,7 @@
       <c r="I35" t="s">
         <v>47</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="J35" s="1" t="s">
         <v>142</v>
       </c>
       <c r="K35">
@@ -2216,7 +2224,7 @@
       <c r="I40" t="s">
         <v>60</v>
       </c>
-      <c r="J40" s="2" t="s">
+      <c r="J40" s="1" t="s">
         <v>143</v>
       </c>
       <c r="K40">
@@ -2253,7 +2261,7 @@
       <c r="I41" t="s">
         <v>63</v>
       </c>
-      <c r="J41" s="2" t="s">
+      <c r="J41" s="1" t="s">
         <v>144</v>
       </c>
       <c r="K41">
@@ -2290,7 +2298,7 @@
       <c r="I42" t="s">
         <v>66</v>
       </c>
-      <c r="J42" s="2" t="s">
+      <c r="J42" s="1" t="s">
         <v>145</v>
       </c>
       <c r="K42">
@@ -2333,6 +2341,9 @@
     <hyperlink ref="J19" r:id="rId19" xr:uid="{589175BE-89C4-4D52-AAFB-C859B358E278}"/>
     <hyperlink ref="J20" r:id="rId20" xr:uid="{A70B7D86-B12D-415C-9FA6-8E7953247930}"/>
     <hyperlink ref="J21" r:id="rId21" xr:uid="{0012A689-3780-4B5A-9A71-79DD9B35A2C2}"/>
+    <hyperlink ref="J30" r:id="rId22" xr:uid="{DADA061F-A70A-4920-A249-6A342CBE0CB1}"/>
+    <hyperlink ref="J31" r:id="rId23" xr:uid="{75354BB3-C417-4890-A98E-4CDEBD18F696}"/>
+    <hyperlink ref="J32" r:id="rId24" xr:uid="{73D34756-E64A-49F1-ADD7-FA46090BE75D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>